<commit_message>
add time simulation and graphic updated accordingly. add second update manual. add var durasiFullSIklus at homepage. clean some code
</commit_message>
<xml_diff>
--- a/data_uji_ekstrem.xlsx
+++ b/data_uji_ekstrem.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\skripsi\idzniskripsi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3654EC-1862-4DE6-BB9C-4D697D833A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="2340" yWindow="2790" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet 1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -46,8 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -65,7 +70,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -105,35 +110,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -144,10 +158,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -185,71 +199,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -277,7 +291,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -300,11 +314,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -313,13 +327,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -329,7 +343,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -338,7 +352,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -347,7 +361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -355,10 +369,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -423,28 +437,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="4.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,185 +482,191 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>8.2</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C2" s="4">
         <v>80</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>54</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>74.25</v>
       </c>
-      <c r="F2" s="4">
-        <v>0.0077</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.0185</v>
-      </c>
-      <c r="H2" s="4">
-        <f>G2-F2</f>
-      </c>
-      <c r="I2" s="4">
+      <c r="F2" s="5">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H2" s="5">
+        <f t="shared" ref="H2:H7" si="0">G2-F2</f>
+        <v>1.0799999999999999E-2</v>
+      </c>
+      <c r="I2" s="5">
         <v>245.5488</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>80</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>52</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>74.33</v>
       </c>
-      <c r="F3" s="4">
-        <v>0.0085</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.0185</v>
-      </c>
-      <c r="H3" s="4">
-        <f>G3-F3</f>
-      </c>
-      <c r="I3" s="4">
+      <c r="F3" s="5">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999985E-3</v>
+      </c>
+      <c r="I3" s="5">
         <v>227.36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>17.4</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="C4" s="4">
         <v>80</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>46</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>74.67</v>
       </c>
-      <c r="F4" s="4">
-        <v>0.011</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.0185</v>
-      </c>
-      <c r="H4" s="4">
-        <f>G4-F4</f>
-      </c>
-      <c r="I4" s="4">
+      <c r="F4" s="5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="I4" s="5">
         <v>170.52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>25.9</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>80</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>41.4</v>
       </c>
-      <c r="E5" s="4">
-        <v>74.79</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.013</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.0185</v>
-      </c>
-      <c r="H5" s="4">
-        <f>G5-F5</f>
-      </c>
-      <c r="I5" s="4">
+      <c r="E5" s="5">
+        <v>74.790000000000006</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="0"/>
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="I5" s="5">
         <v>125.048</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3">
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>31.9</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>80</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>39</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>75.31</v>
       </c>
-      <c r="F6" s="4">
-        <v>0.014</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.0185</v>
-      </c>
-      <c r="H6" s="4">
-        <f>G6-F6</f>
-      </c>
-      <c r="I6" s="4">
+      <c r="F6" s="5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999988E-3</v>
+      </c>
+      <c r="I6" s="5">
         <v>102.312</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>40</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>80</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>36.15</v>
       </c>
-      <c r="E7" s="4">
-        <v>75.1</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.0151</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.0185</v>
-      </c>
-      <c r="H7" s="4">
-        <f>G7-F7</f>
-      </c>
-      <c r="I7" s="4">
-        <v>77.3024</v>
+      <c r="E7" s="5">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="0"/>
+        <v>3.3999999999999985E-3</v>
+      </c>
+      <c r="I7" s="5">
+        <v>77.302400000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>